<commit_message>
Good Point ,try to make print for the AttendanceControls
</commit_message>
<xml_diff>
--- a/AttendanceControls/bin/Debug/salary.xlsx
+++ b/AttendanceControls/bin/Debug/salary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="28800" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
   <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +810,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>